<commit_message>
Elementos de plan de sevicio}
Elementos de plan de sevicio}
</commit_message>
<xml_diff>
--- a/InterProPruebasAutomatizadas/InterProHerramientas/Comunes/DatosPrueba.xlsx
+++ b/InterProPruebasAutomatizadas/InterProHerramientas/Comunes/DatosPrueba.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UsuariosPortal" sheetId="1" r:id="rId1"/>
+    <sheet name="PlanesDeServicio" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
   <si>
     <t>Usuario</t>
   </si>
@@ -82,13 +83,40 @@
   </si>
   <si>
     <t>Sin_Contrasenia</t>
+  </si>
+  <si>
+    <t>NombrePlan</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Tarjeta</t>
+  </si>
+  <si>
+    <t>CostoPlan</t>
+  </si>
+  <si>
+    <t>Servicio1</t>
+  </si>
+  <si>
+    <t>Servicio2</t>
+  </si>
+  <si>
+    <t>Buro</t>
+  </si>
+  <si>
+    <t>PlanBasico</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +134,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -151,11 +186,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -163,9 +199,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Moneda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -446,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,4 +687,105 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="5">
+        <v>16</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
HP Plan de Servicio
</commit_message>
<xml_diff>
--- a/InterProPruebasAutomatizadas/InterProHerramientas/Comunes/DatosPrueba.xlsx
+++ b/InterProPruebasAutomatizadas/InterProHerramientas/Comunes/DatosPrueba.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="38">
   <si>
     <t>Usuario</t>
   </si>
@@ -76,9 +76,6 @@
     <t>juan.valderrama@mobiik.com</t>
   </si>
   <si>
-    <t>00</t>
-  </si>
-  <si>
     <t>Sin_Datos</t>
   </si>
   <si>
@@ -97,16 +94,46 @@
     <t>CostoPlan</t>
   </si>
   <si>
-    <t>Servicio1</t>
-  </si>
-  <si>
-    <t>Servicio2</t>
-  </si>
-  <si>
     <t>Buro</t>
   </si>
   <si>
-    <t>PlanBasico</t>
+    <t>ServicioBuro</t>
+  </si>
+  <si>
+    <t>ServicioTarjeta</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Crear</t>
+  </si>
+  <si>
+    <t>Alta_Exitosa_PlanServicioCamposObligatorios</t>
+  </si>
+  <si>
+    <t>Alta_Exitosa_PlanServicioTodosLosCampos</t>
+  </si>
+  <si>
+    <t>FireFox</t>
+  </si>
+  <si>
+    <t>afd13ccb</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>PBuroTarjetaA</t>
+  </si>
+  <si>
+    <t>PBuroA</t>
+  </si>
+  <si>
+    <t>PTarjetasB</t>
+  </si>
+  <si>
+    <t>PBuroTarjetaB</t>
   </si>
 </sst>
 </file>
@@ -162,7 +189,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -185,13 +212,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -200,6 +238,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -482,17 +523,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
     <col min="4" max="4" width="48" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
@@ -553,7 +594,7 @@
         <v>17</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
@@ -637,7 +678,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>17</v>
@@ -658,7 +699,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="2"/>
@@ -672,6 +713,159 @@
         <v>7</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2">
+        <v>12345679</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="2">
+        <v>12345679</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -684,6 +878,13 @@
     <hyperlink ref="B3" r:id="rId5"/>
     <hyperlink ref="D3" r:id="rId6"/>
     <hyperlink ref="B7" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8"/>
+    <hyperlink ref="B11" r:id="rId9"/>
+    <hyperlink ref="B12" r:id="rId10"/>
+    <hyperlink ref="D9" r:id="rId11"/>
+    <hyperlink ref="B10" r:id="rId12"/>
+    <hyperlink ref="D10" r:id="rId13"/>
+    <hyperlink ref="B14" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -691,27 +892,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="48" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.42578125" customWidth="1"/>
     <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -731,13 +933,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>25</v>
@@ -745,46 +947,352 @@
       <c r="K1" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="5">
+        <v>50</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C3" s="2">
         <v>12345678</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="5">
+        <v>67</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="5">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="5">
         <v>16</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="I4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="5">
+        <v>16</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="5">
+        <v>16</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="5">
+        <v>16</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="5">
+        <v>16</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="5">
+        <v>16</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="5">
+        <v>16</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="D5" r:id="rId3"/>
+    <hyperlink ref="B7" r:id="rId4"/>
+    <hyperlink ref="D7" r:id="rId5"/>
+    <hyperlink ref="B8" r:id="rId6"/>
+    <hyperlink ref="D8" r:id="rId7"/>
+    <hyperlink ref="B6" r:id="rId8"/>
+    <hyperlink ref="D6" r:id="rId9"/>
+    <hyperlink ref="B9" r:id="rId10"/>
+    <hyperlink ref="D9" r:id="rId11"/>
+    <hyperlink ref="B10" r:id="rId12"/>
+    <hyperlink ref="D10" r:id="rId13"/>
+    <hyperlink ref="D3" r:id="rId14"/>
+    <hyperlink ref="B3" r:id="rId15"/>
+    <hyperlink ref="D4" r:id="rId16"/>
+    <hyperlink ref="B4" r:id="rId17"/>
+    <hyperlink ref="B5" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Carga de Datos Preguntas Frecuentes
Carga de Datos Preguntas Frecuentes
</commit_message>
<xml_diff>
--- a/InterProPruebasAutomatizadas/InterProHerramientas/Comunes/DatosPrueba.xlsx
+++ b/InterProPruebasAutomatizadas/InterProHerramientas/Comunes/DatosPrueba.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="UsuariosPortal" sheetId="1" r:id="rId1"/>
     <sheet name="PlanesDeServicio" sheetId="2" r:id="rId2"/>
     <sheet name="Empleados" sheetId="3" r:id="rId3"/>
+    <sheet name="PreguntasFrecuentes" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="86">
   <si>
     <t>Usuario</t>
   </si>
@@ -210,6 +211,75 @@
   </si>
   <si>
     <t>Juan Valderrama</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>Activar</t>
+  </si>
+  <si>
+    <t>Pregunta</t>
+  </si>
+  <si>
+    <t>Respuesta</t>
+  </si>
+  <si>
+    <t>Servicio / Producto</t>
+  </si>
+  <si>
+    <t>Robo de identidad</t>
+  </si>
+  <si>
+    <t>Contacto</t>
+  </si>
+  <si>
+    <t>Quienes somos</t>
+  </si>
+  <si>
+    <t>Tiene dudas sobre el producto</t>
+  </si>
+  <si>
+    <t>Como proteger su identidad</t>
+  </si>
+  <si>
+    <t>Desea contactarnos</t>
+  </si>
+  <si>
+    <t>Informacion de WEPID</t>
+  </si>
+  <si>
+    <t>xxxx</t>
+  </si>
+  <si>
+    <t>TipoPrueba</t>
+  </si>
+  <si>
+    <t>Crea</t>
+  </si>
+  <si>
+    <t>Alta_Exitosa_PreguntaCamposObligatorios</t>
+  </si>
+  <si>
+    <t>Eliminar_Pregunta</t>
+  </si>
+  <si>
+    <t>Editar_Pregunta</t>
+  </si>
+  <si>
+    <t>xxxxxxxx</t>
+  </si>
+  <si>
+    <t>La pregunta sera dada de baja</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>editar</t>
+  </si>
+  <si>
+    <t>Eliminar</t>
   </si>
 </sst>
 </file>
@@ -1229,8 +1299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1514,4 +1584,350 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="31.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
+    <hyperlink ref="D8" r:id="rId7"/>
+    <hyperlink ref="D9" r:id="rId8"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>